<commit_message>
Take out biomass from building electrification
</commit_message>
<xml_diff>
--- a/InputData/bldgs/RBFF/Recipient Buildings Fuel Fractions.xlsx
+++ b/InputData/bldgs/RBFF/Recipient Buildings Fuel Fractions.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Energy Innovation)\EI-PlcyMdl\eps-1.5.0-us-wipD\InputData\bldgs\RBFF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\United States\NEW_US\InputData\bldgs\RBFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE4E3257-D795-4A92-804F-0180AA3862CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25815" windowHeight="11295"/>
+    <workbookView xWindow="9660" yWindow="1080" windowWidth="17205" windowHeight="16065" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -96,7 +97,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -429,10 +430,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -496,13 +499,15 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -566,7 +571,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" s="5">
         <v>1</v>
@@ -741,7 +746,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="5">
         <v>0</v>

</xml_diff>